<commit_message>
IMU board submit, doesn't work
</commit_message>
<xml_diff>
--- a/IMUBoard/JLC_BOM.xlsx
+++ b/IMUBoard/JLC_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\eagle\IMUBoard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4657563F-39D3-4A1C-A18F-A4DD036F4DD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED0305D-3906-42FF-8EFB-B6A751C03E2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="12050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
   <si>
     <t>Comment</t>
   </si>
@@ -185,17 +185,30 @@
   <si>
     <t>C8,C9,C10,C11,C12</t>
   </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>1016-1101-5-ND</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -291,44 +304,47 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -606,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="14.4"/>
@@ -621,7 +637,7 @@
     <col min="5" max="5" width="22.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -637,8 +653,11 @@
       <c r="E1" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="F1" s="6" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -655,7 +674,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16" customHeight="1">
+    <row r="3" spans="1:6" ht="16" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -672,7 +691,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="17" customHeight="1">
+    <row r="4" spans="1:6" ht="17" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -689,7 +708,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
@@ -706,7 +725,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6" s="10" t="s">
         <v>29</v>
       </c>
@@ -723,7 +742,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7" s="10" t="s">
         <v>30</v>
       </c>
@@ -740,7 +759,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8" s="10" t="s">
         <v>38</v>
       </c>
@@ -756,8 +775,11 @@
       <c r="E8" s="10" t="s">
         <v>37</v>
       </c>
+      <c r="F8" s="13" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="A9" s="10" t="s">
         <v>41</v>
       </c>

</xml_diff>